<commit_message>
Validaciones DG, CL, PL
Se están corroborando los ajustes de validaciones por parte de la retroalimentación recibida
</commit_message>
<xml_diff>
--- a/Archivos_excel/01_Retroalimentacion/Formato_retro_PLE (01Agosto2024).xlsx
+++ b/Archivos_excel/01_Retroalimentacion/Formato_retro_PLE (01Agosto2024).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://365inegi-my.sharepoint.com/personal/francisco_deferia_inegi_org_mx/Documents/001_Programacion_FJMD/02_C#/03_App_PLE_INEGI/Archivos_excel/01_Retroalimentacion/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\01_Programacion_FJMD\#C\Aplicativo_PLE_INEGI\Archivos_excel\01_Retroalimentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="134" documentId="8_{AA7C9837-32C6-4D57-A061-F3863BBCE6D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3BE229E5-8235-4A99-867E-9C810D8D300A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{472A035F-F134-45F6-9148-D817120AB8E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{7D6F1DB5-4C81-46D9-BE7A-7D2828049709}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{7D6F1DB5-4C81-46D9-BE7A-7D2828049709}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="100">
   <si>
     <t>Hoja</t>
   </si>
@@ -369,6 +369,12 @@
   </si>
   <si>
     <t>Doctorado</t>
+  </si>
+  <si>
+    <t>Completa</t>
+  </si>
+  <si>
+    <t>falta una parte</t>
   </si>
 </sst>
 </file>
@@ -601,7 +607,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -971,10 +997,10 @@
   <dimension ref="A1:L58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E53" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C59" sqref="C59"/>
+      <selection pane="bottomRight" activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1119,12 +1145,16 @@
       <c r="D6" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="E6" s="19"/>
+      <c r="E6" s="19" t="s">
+        <v>98</v>
+      </c>
       <c r="F6" s="19"/>
       <c r="G6" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="H6" s="12"/>
+      <c r="H6" s="12" t="s">
+        <v>98</v>
+      </c>
       <c r="I6" s="12"/>
       <c r="J6" s="13"/>
       <c r="K6" s="13"/>
@@ -1141,7 +1171,9 @@
       <c r="D7" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="18"/>
+      <c r="E7" s="18" t="s">
+        <v>98</v>
+      </c>
       <c r="F7" s="18"/>
       <c r="G7" s="18"/>
       <c r="H7" s="10"/>
@@ -1159,7 +1191,9 @@
       <c r="D8" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="E8" s="18"/>
+      <c r="E8" s="18" t="s">
+        <v>98</v>
+      </c>
       <c r="F8" s="18"/>
       <c r="G8" s="18"/>
       <c r="H8" s="10"/>
@@ -1177,7 +1211,9 @@
       <c r="D9" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="18"/>
+      <c r="E9" s="18" t="s">
+        <v>98</v>
+      </c>
       <c r="F9" s="18"/>
       <c r="G9" s="18"/>
       <c r="H9" s="10"/>
@@ -1195,7 +1231,9 @@
       <c r="D10" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="18"/>
+      <c r="E10" s="18" t="s">
+        <v>98</v>
+      </c>
       <c r="F10" s="18"/>
       <c r="G10" s="18"/>
       <c r="H10" s="10"/>
@@ -1213,12 +1251,16 @@
       <c r="D11" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="E11" s="18"/>
+      <c r="E11" s="18" t="s">
+        <v>98</v>
+      </c>
       <c r="F11" s="18"/>
       <c r="G11" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="H11" s="10"/>
+      <c r="H11" s="10" t="s">
+        <v>98</v>
+      </c>
       <c r="I11" s="10"/>
       <c r="L11" s="16"/>
     </row>
@@ -1233,12 +1275,16 @@
       <c r="D12" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="18"/>
+      <c r="E12" s="18" t="s">
+        <v>98</v>
+      </c>
       <c r="F12" s="18"/>
       <c r="G12" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="H12" s="10"/>
+      <c r="H12" s="10" t="s">
+        <v>98</v>
+      </c>
       <c r="I12" s="10"/>
       <c r="L12" s="16"/>
     </row>
@@ -1255,7 +1301,9 @@
       <c r="D13" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="19"/>
+      <c r="E13" s="19" t="s">
+        <v>98</v>
+      </c>
       <c r="F13" s="19"/>
       <c r="G13" s="19"/>
       <c r="H13" s="12"/>
@@ -1275,7 +1323,9 @@
       <c r="D14" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E14" s="18"/>
+      <c r="E14" s="18" t="s">
+        <v>98</v>
+      </c>
       <c r="F14" s="18"/>
       <c r="G14" s="18"/>
       <c r="H14" s="10"/>
@@ -1293,7 +1343,9 @@
       <c r="D15" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="18"/>
+      <c r="E15" s="18" t="s">
+        <v>98</v>
+      </c>
       <c r="F15" s="18"/>
       <c r="G15" s="18" t="s">
         <v>62</v>
@@ -1313,7 +1365,9 @@
       <c r="D16" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="18"/>
+      <c r="E16" s="18" t="s">
+        <v>98</v>
+      </c>
       <c r="F16" s="18"/>
       <c r="G16" s="18"/>
       <c r="H16" s="10"/>
@@ -1385,7 +1439,9 @@
       <c r="D20" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E20" s="18"/>
+      <c r="E20" s="18" t="s">
+        <v>98</v>
+      </c>
       <c r="F20" s="18"/>
       <c r="G20" s="18"/>
       <c r="L20" s="16"/>
@@ -1401,7 +1457,9 @@
       <c r="D21" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="E21" s="18"/>
+      <c r="E21" s="18" t="s">
+        <v>98</v>
+      </c>
       <c r="F21" s="18"/>
       <c r="G21" s="18" t="s">
         <v>63</v>
@@ -1419,7 +1477,9 @@
       <c r="D22" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="E22" s="18"/>
+      <c r="E22" s="18" t="s">
+        <v>98</v>
+      </c>
       <c r="F22" s="18"/>
       <c r="G22" s="18" t="s">
         <v>83</v>
@@ -1437,8 +1497,12 @@
       <c r="D23" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
+      <c r="E23" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>99</v>
+      </c>
       <c r="G23" s="18"/>
       <c r="L23" s="16"/>
     </row>
@@ -1453,8 +1517,12 @@
       <c r="D24" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
+      <c r="E24" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>99</v>
+      </c>
       <c r="G24" s="18"/>
       <c r="L24" s="16"/>
     </row>
@@ -1469,8 +1537,12 @@
       <c r="D25" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
+      <c r="E25" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>99</v>
+      </c>
       <c r="G25" s="18"/>
       <c r="L25" s="16"/>
     </row>
@@ -1485,8 +1557,12 @@
       <c r="D26" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
+      <c r="E26" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>99</v>
+      </c>
       <c r="G26" s="18"/>
       <c r="L26" s="16"/>
     </row>
@@ -1501,7 +1577,9 @@
       <c r="D27" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E27" s="18"/>
+      <c r="E27" s="18" t="s">
+        <v>98</v>
+      </c>
       <c r="F27" s="18"/>
       <c r="G27" s="18"/>
       <c r="L27" s="16"/>
@@ -1517,7 +1595,9 @@
       <c r="D28" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E28" s="18"/>
+      <c r="E28" s="18" t="s">
+        <v>98</v>
+      </c>
       <c r="F28" s="18"/>
       <c r="G28" s="18" t="s">
         <v>84</v>
@@ -1535,7 +1615,9 @@
       <c r="D29" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E29" s="18"/>
+      <c r="E29" s="18" t="s">
+        <v>98</v>
+      </c>
       <c r="F29" s="18"/>
       <c r="G29" s="18" t="s">
         <v>85</v>
@@ -1553,7 +1635,9 @@
       <c r="D30" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="E30" s="18"/>
+      <c r="E30" s="18" t="s">
+        <v>98</v>
+      </c>
       <c r="F30" s="18"/>
       <c r="G30" s="18"/>
       <c r="L30" s="16"/>
@@ -1569,8 +1653,12 @@
       <c r="D31" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
+      <c r="E31" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="F31" s="18" t="s">
+        <v>99</v>
+      </c>
       <c r="G31" s="18" t="s">
         <v>67</v>
       </c>
@@ -1587,8 +1675,12 @@
       <c r="D32" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
+      <c r="E32" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="F32" s="18" t="s">
+        <v>99</v>
+      </c>
       <c r="G32" s="18"/>
       <c r="L32" s="16"/>
     </row>
@@ -2032,11 +2124,11 @@
     <mergeCell ref="A13:A17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="E3:E17">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <conditionalFormatting sqref="E3:E517">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Completa"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Pendiente"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>